<commit_message>
feat: move table location; wrap cell containing book name and resize
resize cells containing long book names, over 30 chars
</commit_message>
<xml_diff>
--- a/forms-librarie-app/bin/Debug/carti_favorite.xlsx
+++ b/forms-librarie-app/bin/Debug/carti_favorite.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t xml:space="preserve">Cărți favorite</t>
   </si>
@@ -41,76 +41,97 @@
     <t xml:space="preserve">Preț</t>
   </si>
   <si>
-    <t xml:space="preserve">Kathie si hipopotamul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vargas Llosa Mario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curtea Veche</t>
+    <t xml:space="preserve">Drumul spre Biserica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dabija Nicolae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789975444606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venus ia foc Marte e de gheata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gray John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vremea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictiune,mistica,fantazy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789736455575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adobe InDesign CC. Официальный учебный курс (+ CD-ROM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Круз Дж.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Эксмо</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer,internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9785699696598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Povesti in romana si germana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sojka Anna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flamingo</t>
   </si>
   <si>
     <t xml:space="preserve">2010</t>
   </si>
   <si>
-    <t xml:space="preserve">264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proza , Dramaturgie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9786065880702</t>
-  </si>
-  <si>
-    <t xml:space="preserve">132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drumul spre Biserica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dabija Nicolae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789975444606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe InDesign CC. Официальный учебный курс (+ CD-ROM)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Круз Дж.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Эксмо</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer,internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9785699696598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">740</t>
+    <t xml:space="preserve">104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poezii,povesti,povestiri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789738873308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">174</t>
   </si>
   <si>
     <t xml:space="preserve">Dictionar Oxford de istorie universala contemporana (2 vol.)</t>
@@ -243,7 +264,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="96">
+  <borders count="97">
     <border>
       <left/>
       <right/>
@@ -629,11 +650,17 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment/>
@@ -1013,6 +1040,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment vertical="center"/>
+      <protection locked="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="1"/>
     </xf>
   </cellXfs>
@@ -1044,170 +1075,212 @@
     <col min="8" max="8" width="8" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="8" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="8" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="D3" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>0</v>
+      <c r="A3" s="1"/>
+      <c r="B3" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="90" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="D4" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="85" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="90" t="s">
-        <v>8</v>
+      <c r="A4" s="1"/>
+      <c r="B4" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="95" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="95" t="s">
+        <v>18</v>
+      </c>
       <c r="D5" s="95" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E5" s="95" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" s="95" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G5" s="95" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H5" s="95" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I5" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="95" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="95" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" ht="65" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>25</v>
+      </c>
       <c r="D6" s="95" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E6" s="95" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F6" s="95" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G6" s="95" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H6" s="95" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I6" s="95" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="95" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="95" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="1"/>
+      <c r="B7" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>33</v>
+      </c>
       <c r="D7" s="95" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E7" s="95" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F7" s="95" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G7" s="95" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H7" s="95" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="95" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="95" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" ht="65" customHeight="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>41</v>
+      </c>
       <c r="D8" s="95" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E8" s="95" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F8" s="95" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G8" s="95" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H8" s="95" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="95" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="95" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells>
-    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="default" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>

<commit_message>
feat: move table location; add wrapping to book name
</commit_message>
<xml_diff>
--- a/forms-librarie-app/bin/Debug/carti_favorite.xlsx
+++ b/forms-librarie-app/bin/Debug/carti_favorite.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
   <si>
     <t xml:space="preserve">Cărți favorite</t>
   </si>
@@ -41,76 +41,97 @@
     <t xml:space="preserve">Preț</t>
   </si>
   <si>
-    <t xml:space="preserve">Kathie si hipopotamul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vargas Llosa Mario</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curtea Veche</t>
+    <t xml:space="preserve">Drumul spre Biserica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dabija Nicolae</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Europress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789975444606</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venus ia foc Marte e de gheata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gray John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vremea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictiune,mistica,fantazy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789736455575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adobe InDesign CC. Официальный учебный курс (+ CD-ROM)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Круз Дж.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Эксмо</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">496</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Computer,internet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9785699696598</t>
+  </si>
+  <si>
+    <t xml:space="preserve">740</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Povesti in romana si germana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sojka Anna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flamingo</t>
   </si>
   <si>
     <t xml:space="preserve">2010</t>
   </si>
   <si>
-    <t xml:space="preserve">264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proza , Dramaturgie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9786065880702</t>
-  </si>
-  <si>
-    <t xml:space="preserve">132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drumul spre Biserica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dabija Nicolae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789975444606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe InDesign CC. Официальный учебный курс (+ CD-ROM)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Круз Дж.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Эксмо</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer,internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9785699696598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">740</t>
+    <t xml:space="preserve">104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poezii,povesti,povestiri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789738873308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">174</t>
   </si>
   <si>
     <t xml:space="preserve">Dictionar Oxford de istorie universala contemporana (2 vol.)</t>
@@ -243,7 +264,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="96">
+  <borders count="97">
     <border>
       <left/>
       <right/>
@@ -629,11 +650,17 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment/>
@@ -1013,6 +1040,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment vertical="center"/>
+      <protection locked="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
+      <alignment vertical="center" wrapText="1"/>
       <protection locked="1"/>
     </xf>
   </cellXfs>
@@ -1044,170 +1075,212 @@
     <col min="8" max="8" width="8" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="8" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="8" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="1"/>
+      <c r="B2" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="D3" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>0</v>
+      <c r="A3" s="1"/>
+      <c r="B3" s="83" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="85" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="88" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="90" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="D4" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="84" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="85" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="86" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" s="88" t="s">
-        <v>6</v>
-      </c>
-      <c r="J4" s="89" t="s">
-        <v>7</v>
-      </c>
-      <c r="K4" s="90" t="s">
-        <v>8</v>
+      <c r="A4" s="1"/>
+      <c r="B4" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="95" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="95" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="95" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="95" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="95" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="95" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="1"/>
+      <c r="B5" s="95" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="95" t="s">
+        <v>18</v>
+      </c>
       <c r="D5" s="95" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E5" s="95" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" s="95" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="G5" s="95" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="H5" s="95" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="I5" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" s="95" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="95" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="6" ht="15" customHeight="1">
+    <row r="6" ht="65" customHeight="1">
+      <c r="A6" s="1"/>
+      <c r="B6" s="96" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>25</v>
+      </c>
       <c r="D6" s="95" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E6" s="95" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F6" s="95" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G6" s="95" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="H6" s="95" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I6" s="95" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="95" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="95" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="1"/>
+      <c r="B7" s="95" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>33</v>
+      </c>
       <c r="D7" s="95" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E7" s="95" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F7" s="95" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="G7" s="95" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H7" s="95" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="95" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="95" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
-    <row r="8" ht="15" customHeight="1">
+    <row r="8" ht="65" customHeight="1">
+      <c r="A8" s="1"/>
+      <c r="B8" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="95" t="s">
+        <v>41</v>
+      </c>
       <c r="D8" s="95" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E8" s="95" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F8" s="95" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G8" s="95" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H8" s="95" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="I8" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="J8" s="95" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="95" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells>
-    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" orientation="default" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>

<commit_message>
feat: implement book addition and removal for admin interface
</commit_message>
<xml_diff>
--- a/forms-librarie-app/bin/Debug/carti_favorite.xlsx
+++ b/forms-librarie-app/bin/Debug/carti_favorite.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t xml:space="preserve">Cărți favorite</t>
   </si>
@@ -41,39 +41,42 @@
     <t xml:space="preserve">Preț</t>
   </si>
   <si>
-    <t xml:space="preserve">Drumul spre Biserica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dabija Nicolae</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Europress</t>
+    <t xml:space="preserve">In apararea pietelor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Lucian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Curtea Veche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">416</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Economie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9786065883239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Venus ia foc Marte e de gheata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gray John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vremea</t>
   </si>
   <si>
     <t xml:space="preserve">2013</t>
   </si>
   <si>
-    <t xml:space="preserve">312</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Roman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789975444606</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venus ia foc Marte e de gheata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gray John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vremea</t>
-  </si>
-  <si>
     <t xml:space="preserve">232</t>
   </si>
   <si>
@@ -84,78 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe InDesign CC. Официальный учебный курс (+ CD-ROM)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Круз Дж.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Эксмо</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">496</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Computer,internet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9785699696598</t>
-  </si>
-  <si>
-    <t xml:space="preserve">740</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Povesti in romana si germana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sojka Anna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flamingo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poezii,povesti,povestiri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789738873308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dictionar Oxford de istorie universala contemporana (2 vol.)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palmowski J.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">504</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specialitate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789735715519</t>
-  </si>
-  <si>
-    <t xml:space="preserve">395</t>
   </si>
 </sst>
 </file>
@@ -264,7 +195,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="97">
+  <borders count="96">
     <border>
       <left/>
       <right/>
@@ -650,17 +581,11 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment/>
@@ -1040,10 +965,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment vertical="center"/>
-      <protection locked="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
-      <alignment vertical="center" wrapText="1"/>
       <protection locked="1"/>
     </xf>
   </cellXfs>
@@ -1077,19 +998,7 @@
     <col min="10" max="10" width="8" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-    </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="1"/>
       <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1025,6 @@
       </c>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="1"/>
       <c r="B3" s="83" t="s">
         <v>1</v>
       </c>
@@ -1143,7 +1051,6 @@
       </c>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="1"/>
       <c r="B4" s="95" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1077,6 @@
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="1"/>
       <c r="B5" s="95" t="s">
         <v>17</v>
       </c>
@@ -1181,100 +1087,19 @@
         <v>19</v>
       </c>
       <c r="E5" s="95" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F5" s="95" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G5" s="95" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H5" s="95" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5" s="95" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" ht="65" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="96" t="s">
         <v>24</v>
-      </c>
-      <c r="C6" s="95" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="95" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="95" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="95" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="95" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="95" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="95" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="95" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="95" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" s="95" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="95" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="95" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="95" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="95" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="95" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" ht="65" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="96" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="95" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="95" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="95" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="95" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="95" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="95" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: fix accessing page without log in
</commit_message>
<xml_diff>
--- a/forms-librarie-app/bin/Debug/carti_favorite.xlsx
+++ b/forms-librarie-app/bin/Debug/carti_favorite.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t xml:space="preserve">Cărți favorite</t>
   </si>
@@ -40,54 +40,6 @@
   <si>
     <t xml:space="preserve">Preț</t>
   </si>
-  <si>
-    <t xml:space="preserve">In apararea pietelor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Lucian</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Curtea Veche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">416</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Economie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9786065883239</t>
-  </si>
-  <si>
-    <t xml:space="preserve">185</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venus ia foc Marte e de gheata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gray John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vremea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fictiune,mistica,fantazy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789736455575</t>
-  </si>
-  <si>
-    <t xml:space="preserve">235</t>
-  </si>
 </sst>
 </file>
 
@@ -195,7 +147,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="96">
+  <borders count="91">
     <border>
       <left/>
       <right/>
@@ -557,35 +509,11 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
-    <border>
-      <left style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment/>
@@ -945,26 +873,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
       <alignment shrinkToFit="1"/>
-      <protection locked="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
-      <alignment/>
-      <protection locked="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
-      <alignment/>
-      <protection locked="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
-      <alignment/>
-      <protection locked="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
-      <alignment/>
-      <protection locked="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0">
-      <alignment vertical="center"/>
       <protection locked="1"/>
     </xf>
   </cellXfs>
@@ -1050,58 +958,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="15" customHeight="1">
-      <c r="B4" s="95" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="95" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="95" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="95" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="95" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="95" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="95" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" ht="15" customHeight="1">
-      <c r="B5" s="95" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="95" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="95" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="95" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="95" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="95" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="95" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="95" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells>

</xml_diff>

<commit_message>
refactor: replace UTC date with local timezone date
</commit_message>
<xml_diff>
--- a/forms-librarie-app/bin/Debug/carti_favorite.xlsx
+++ b/forms-librarie-app/bin/Debug/carti_favorite.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
   <si>
     <t xml:space="preserve">Librarius</t>
   </si>
@@ -44,102 +44,60 @@
     <t xml:space="preserve">Preț</t>
   </si>
   <si>
-    <t xml:space="preserve">Povesti in romana si germana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sojka Anna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flamingo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">104</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poezii,povesti,povestiri</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789738873308</t>
-  </si>
-  <si>
-    <t xml:space="preserve">174</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kathie si hipopotamul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vargas Llosa Mario</t>
+    <t xml:space="preserve">Venus ia foc Marte e de gheata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gray John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vremea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fictiune,mistica,fantazy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789736455575</t>
+  </si>
+  <si>
+    <t xml:space="preserve">235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cu ochii mintii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashner James</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trei</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9786067198157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In apararea pietelor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Lucian</t>
   </si>
   <si>
     <t xml:space="preserve">Curtea Veche</t>
   </si>
   <si>
-    <t xml:space="preserve">264</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Proza , Dramaturgie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9786065880702</t>
-  </si>
-  <si>
-    <t xml:space="preserve">132</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Venus ia foc Marte e de gheata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gray John</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vremea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fictiune,mistica,fantazy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9789736455575</t>
-  </si>
-  <si>
-    <t xml:space="preserve">235</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cu ochii mintii</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dashner James</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trei</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">216</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9786067198157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">170</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In apararea pietelor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Lucian</t>
-  </si>
-  <si>
     <t xml:space="preserve">2012</t>
   </si>
   <si>
@@ -155,6 +113,30 @@
     <t xml:space="preserve">185</t>
   </si>
   <si>
+    <t xml:space="preserve">Cele 12 elemente ale managementului performant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wagner R.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9789737241887</t>
+  </si>
+  <si>
+    <t xml:space="preserve">155</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adobe InDesign CC. Официальный учебный курс (+ CD-ROM)</t>
   </si>
   <si>
@@ -179,25 +161,7 @@
     <t xml:space="preserve">740</t>
   </si>
   <si>
-    <t xml:space="preserve">Щенок Элфи или Не хочу быть один!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Вебб Х.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">144</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Literatura pentru copii 7+</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9785699711932</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data exportării: 05/20/2022 1:54</t>
+    <t xml:space="preserve">Data exportării: 05/22/2022 14:05</t>
   </si>
 </sst>
 </file>
@@ -1279,13 +1243,13 @@
         <v>20</v>
       </c>
       <c r="E7" s="98" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F7" s="98" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="98" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="H7" s="98" t="s">
         <v>23</v>
@@ -1321,9 +1285,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" ht="15" customHeight="1">
+    <row r="9" ht="65" customHeight="1">
       <c r="A9" s="1"/>
-      <c r="B9" s="98" t="s">
+      <c r="B9" s="99" t="s">
         <v>33</v>
       </c>
       <c r="C9" s="98" t="s">
@@ -1339,101 +1303,47 @@
         <v>37</v>
       </c>
       <c r="G9" s="98" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="H9" s="98" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I9" s="98" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
-    <row r="10" ht="15" customHeight="1">
+    <row r="10" ht="65" customHeight="1">
       <c r="A10" s="1"/>
-      <c r="B10" s="98" t="s">
-        <v>40</v>
+      <c r="B10" s="99" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="98" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="98" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="E10" s="98" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="F10" s="98" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="G10" s="98" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H10" s="98" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="I10" s="98" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="11" ht="65" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="99" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="98" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="98" t="s">
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13" ht="15" customHeight="1">
+      <c r="B13" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E11" s="98" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="G11" s="98" t="s">
-        <v>52</v>
-      </c>
-      <c r="H11" s="98" t="s">
-        <v>53</v>
-      </c>
-      <c r="I11" s="98" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" ht="65" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="98" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="98" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="98" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="98" t="s">
-        <v>57</v>
-      </c>
-      <c r="G12" s="98" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" s="98" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="98" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15" ht="15" customHeight="1">
-      <c r="B15" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>